<commit_message>
save data in excel
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,396 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Names</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Prices</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>The Legend of Zelda: Ocarina of Time</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>91,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Super Mario Galaxy</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>91,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Super Mario Galaxy 2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>91,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Metroid Prime</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>89,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Super Mario Odyssey</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>89,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Halo: Combat Evolved</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>87,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>The House in Fata Morgana - Dreams of the Revenants Edition -</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>83,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>NFL 2K1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>62,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Uncharted 2: Among Thieves</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>88,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Tekken 3</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>91,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>The Legend of Zelda: The Wind Waker</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>90,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Gran Turismo</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>86,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Metal Gear Solid 2: Sons of Liberty</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>88,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Grand Theft Auto Double Pack</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>81,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Baldur's Gate II: Shadows of Amn</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>91,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Tetris Effect: Connected</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>88,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>The Legend of Zelda Collector's Edition</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>89,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Gran Turismo 3: A-Spec</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>84,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>The Legend of Zelda: A Link to the Past</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>90,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>The Legend of Zelda: Majora's Mask</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>91,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>The Last of Us</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>92,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Persona 5 Royal</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>84,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>The Last of Us Remastered</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>92,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>The Legend of Zelda: Ocarina of Time 3D</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>90,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Chrono Cross</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>88,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Gears of War</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>84,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Sid Meier's Civilization II</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>88,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Halo 3</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>81,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Ninja Gaiden Black</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>88,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Super Mario Advance 4: Super Mario Bros. 3</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>89,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Jet Grind Radio</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>83,99 €</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Grim Fandango</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>91,99 €</t>
         </is>
       </c>
     </row>

</xml_diff>